<commit_message>
Runned first tests, working, to be improved
</commit_message>
<xml_diff>
--- a/dokumentácia/assets/data.xlsx
+++ b/dokumentácia/assets/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\STUFIIT\3. semester\UI\3. zadanie\dokumentácia\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC5675E-2DFB-414C-B0AE-996E5A31B042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01EFD6B-6BE7-4767-ADA7-D294A72040EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{065B6F7D-CFB5-4F11-A3D6-C4BB6CDB67F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{065B6F7D-CFB5-4F11-A3D6-C4BB6CDB67F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>CONFIG</t>
   </si>
@@ -58,35 +58,69 @@
     <t>Vyriešených</t>
   </si>
   <si>
-    <t>Priemerný čas vyriešených</t>
-  </si>
-  <si>
     <t>Dáta</t>
   </si>
   <si>
-    <t>68.86</t>
-  </si>
-  <si>
     <t>Priemerná konečná generácia</t>
   </si>
   <si>
-    <t>4100.</t>
-  </si>
-  <si>
     <t>ČAS</t>
   </si>
   <si>
     <t>GENERÁCIA RIEŠENIA</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>NEDOKONČIL</t>
+  </si>
+  <si>
+    <t>Priemerný čas vyriešených (s)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -113,8 +147,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
@@ -429,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCF5D6F1-2909-479D-94F6-686CCBB48BF7}">
-  <dimension ref="A2:C14"/>
+  <dimension ref="A2:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,77 +493,192 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>100</v>
       </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>100000</v>
-      </c>
+      <c r="B5" s="2">
+        <v>10000</v>
+      </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>2</v>
       </c>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>20</v>
       </c>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>60</v>
       </c>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1">
+        <f>AVERAGE(B14:B20)</f>
+        <v>23.252857142857142</v>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2">
+        <f>AVERAGE(C14:C20)</f>
+        <v>2622.4285714285716</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
         <v>12</v>
       </c>
+      <c r="B14" s="1">
+        <v>8.83</v>
+      </c>
+      <c r="C14" s="2">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>6.98</v>
+      </c>
+      <c r="C15" s="2">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>11.02</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>11.49</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="1">
+        <v>65.34</v>
+      </c>
+      <c r="C18" s="2">
+        <v>7589</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>9.94</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>49.17</v>
+      </c>
+      <c r="C20" s="2">
+        <v>5543</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>